<commit_message>
Muokattu excelin isot alkukirjaimet
</commit_message>
<xml_diff>
--- a/Tietokannan suunnittelu.xlsx
+++ b/Tietokannan suunnittelu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://haagahelia.sharepoint.com/teams/Ohjelmistoprojekti1-Tiimi/Jaetut asiakirjat/General/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickl\Desktop\TicketGuru\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1941" documentId="13_ncr:1_{FFDF21D4-6F73-4F27-87CE-9BBBED5B2CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10632018-5EAD-4329-AC54-890B37DDC7C1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9133F710-44DD-439A-ACAF-99F15F3F317F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="2475" windowWidth="15345" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1545" yWindow="870" windowWidth="17940" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toinen versio" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="55">
   <si>
     <t>PK</t>
   </si>
@@ -114,30 +114,6 @@
     <t>Events</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Place</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Role</t>
-  </si>
-  <si>
     <t>Roles</t>
   </si>
   <si>
@@ -160,42 +136,6 @@
   </si>
   <si>
     <t>Login</t>
-  </si>
-  <si>
-    <t>EventId</t>
-  </si>
-  <si>
-    <t>EventName</t>
-  </si>
-  <si>
-    <t>TicketCount</t>
-  </si>
-  <si>
-    <t>VenueId</t>
-  </si>
-  <si>
-    <t>StreetAddress</t>
-  </si>
-  <si>
-    <t>PostalCode</t>
-  </si>
-  <si>
-    <t>CityId</t>
-  </si>
-  <si>
-    <t>PostOffice</t>
-  </si>
-  <si>
-    <t>TicketId</t>
-  </si>
-  <si>
-    <t>TicketTypeId</t>
-  </si>
-  <si>
-    <t>RoleId</t>
-  </si>
-  <si>
-    <t>TicketType</t>
   </si>
   <si>
     <t>ticketTypeId</t>
@@ -732,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -763,42 +703,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -816,31 +720,11 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -855,7 +739,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -876,11 +760,65 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2635,7 +2573,7 @@
   <dimension ref="B1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="J25" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2661,22 +2599,22 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="24"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
-      <c r="J2" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="24"/>
+      <c r="F2" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="50"/>
+      <c r="H2" s="51"/>
+      <c r="J2" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="50"/>
+      <c r="L2" s="51"/>
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
@@ -2684,7 +2622,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -2693,7 +2631,7 @@
         <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H3" t="s">
         <v>6</v>
@@ -2702,18 +2640,18 @@
         <v>18</v>
       </c>
       <c r="K3" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="L3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="22" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -2722,7 +2660,7 @@
         <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
         <v>8</v>
@@ -2731,7 +2669,7 @@
         <v>10</v>
       </c>
       <c r="K4" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -2742,7 +2680,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -2751,7 +2689,7 @@
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="H5" t="s">
         <v>8</v>
@@ -2760,7 +2698,7 @@
         <v>10</v>
       </c>
       <c r="K5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="L5" t="s">
         <v>4</v>
@@ -2771,7 +2709,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -2782,7 +2720,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -2791,7 +2729,7 @@
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -2799,18 +2737,18 @@
     </row>
     <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
+      <c r="B10" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="53"/>
+      <c r="D10" s="54"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
@@ -2821,7 +2759,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -2832,7 +2770,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>17</v>
@@ -2843,7 +2781,7 @@
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
@@ -2854,7 +2792,7 @@
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
@@ -2863,18 +2801,18 @@
     </row>
     <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="27"/>
+      <c r="B17" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="53"/>
+      <c r="D17" s="54"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
@@ -2885,28 +2823,28 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D19" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="23"/>
-      <c r="H19" s="24"/>
-      <c r="J19" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="K19" s="23"/>
-      <c r="L19" s="24"/>
+      <c r="F19" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="50"/>
+      <c r="H19" s="51"/>
+      <c r="J19" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="50"/>
+      <c r="L19" s="51"/>
     </row>
     <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F20" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G20" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="H20" t="s">
         <v>22</v>
@@ -2915,23 +2853,23 @@
         <v>18</v>
       </c>
       <c r="K20" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="L20" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="21" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="27"/>
+      <c r="B21" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="53"/>
+      <c r="D21" s="54"/>
       <c r="F21" t="s">
         <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H21" t="s">
         <v>23</v>
@@ -2940,7 +2878,7 @@
         <v>10</v>
       </c>
       <c r="K21" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="L21" t="s">
         <v>23</v>
@@ -2951,7 +2889,7 @@
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
         <v>19</v>
@@ -2960,7 +2898,7 @@
         <v>20</v>
       </c>
       <c r="G22" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="H22" t="s">
         <v>8</v>
@@ -2971,7 +2909,7 @@
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
         <v>17</v>
@@ -2979,68 +2917,68 @@
     </row>
     <row r="25" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F26" s="35" t="s">
+      <c r="F26" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="G26" s="36" t="s">
+      <c r="G26" s="24" t="s">
         <v>1</v>
       </c>
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F27" s="37" t="s">
+      <c r="F27" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G27" s="38" t="s">
+      <c r="G27" s="26" t="s">
         <v>3</v>
       </c>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F28" s="37" t="s">
+      <c r="F28" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G28" s="38" t="s">
+      <c r="G28" s="26" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F29" s="37" t="s">
+      <c r="F29" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G29" s="38" t="s">
+      <c r="G29" s="26" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F30" s="37" t="s">
+      <c r="F30" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="38" t="s">
+      <c r="G30" s="26" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F31" s="37" t="s">
+      <c r="F31" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G31" s="38" t="s">
+      <c r="G31" s="26" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F32" s="37" t="s">
+      <c r="F32" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="G32" s="38" t="s">
+      <c r="G32" s="26" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="33" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F33" s="39" t="s">
+      <c r="F33" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="G33" s="40" t="s">
+      <c r="G33" s="28" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3072,10 +3010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77066A0C-FE6B-41C8-82EA-ABF9313DC4DB}">
-  <dimension ref="A2:P46"/>
+  <dimension ref="B2:O46"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3103,384 +3041,313 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="47"/>
+      <c r="B2" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="57"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="21"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
       <c r="O3" s="15"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="16"/>
-      <c r="C4" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
+      <c r="C4" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="62"/>
+      <c r="E4" s="63"/>
+      <c r="G4" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="62"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="29"/>
       <c r="O4" s="17"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="16"/>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="37" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="41"/>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="37" t="s">
         <v>18</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="I5" s="58" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
       <c r="O5" s="17"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="16"/>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="60" t="s">
+      <c r="D6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="41"/>
-      <c r="G6" s="59" t="s">
+      <c r="G6" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" s="60" t="s">
+      <c r="H6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
       <c r="O6" s="17"/>
     </row>
     <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="16"/>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="62" t="s">
-        <v>55</v>
+      <c r="D7" s="42" t="s">
+        <v>35</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="41"/>
-      <c r="G7" s="61" t="s">
+      <c r="G7" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="63" t="s">
-        <v>53</v>
+      <c r="H7" s="43" t="s">
+        <v>33</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41"/>
       <c r="O7" s="17"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="16"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
+      <c r="F8" s="29"/>
       <c r="O8" s="17"/>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="16"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
       <c r="O9" s="17"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="16"/>
-      <c r="C10" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="32"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="28" t="s">
+      <c r="C10" s="61" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="62"/>
+      <c r="E10" s="63"/>
+      <c r="G10" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="65"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="M10" s="29"/>
-      <c r="N10" s="30"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="63"/>
       <c r="O10" s="17"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="16"/>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="37" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="41"/>
-      <c r="G11" s="57" t="s">
+      <c r="G11" s="37" t="s">
         <v>18</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="I11" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="41"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="57" t="s">
+      <c r="L11" s="37" t="s">
         <v>18</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="N11" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="N11" s="38" t="s">
         <v>6</v>
       </c>
       <c r="O11" s="17"/>
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="16"/>
-      <c r="C12" s="61" t="s">
+      <c r="C12" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="62" t="s">
-        <v>57</v>
+      <c r="D12" s="42" t="s">
+        <v>37</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="41"/>
-      <c r="G12" s="59" t="s">
+      <c r="G12" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="I12" s="60" t="s">
+      <c r="H12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="59" t="s">
+      <c r="L12" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="M12" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="N12" s="60" t="s">
+      <c r="M12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="N12" s="40" t="s">
         <v>16</v>
       </c>
       <c r="O12" s="17"/>
     </row>
     <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="16"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="59" t="s">
+      <c r="G13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="I13" s="60" t="s">
+      <c r="H13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="59" t="s">
+      <c r="L13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="M13" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="N13" s="60" t="s">
+      <c r="M13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="N13" s="40" t="s">
         <v>12</v>
       </c>
       <c r="O13" s="17"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="16"/>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="65"/>
+      <c r="E14" s="66"/>
+      <c r="G14" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="32"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="59" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" s="60" t="s">
+      <c r="I14" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="59" t="s">
+      <c r="L14" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="M14" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="N14" s="60" t="s">
+      <c r="M14" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="N14" s="40" t="s">
         <v>8</v>
       </c>
       <c r="O14" s="17"/>
     </row>
     <row r="15" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="16"/>
-      <c r="C15" s="57" t="s">
+      <c r="C15" s="37" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="41"/>
-      <c r="G15" s="61" t="s">
+      <c r="G15" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="63" t="s">
-        <v>58</v>
+      <c r="H15" s="43" t="s">
+        <v>38</v>
       </c>
       <c r="I15" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="59" t="s">
+      <c r="L15" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="M15" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="N15" s="60" t="s">
+      <c r="M15" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="N15" s="40" t="s">
         <v>8</v>
       </c>
       <c r="O15" s="17"/>
     </row>
     <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="16"/>
-      <c r="C16" s="61" t="s">
+      <c r="C16" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="62" t="s">
-        <v>59</v>
+      <c r="D16" s="42" t="s">
+        <v>39</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="61"/>
-      <c r="M16" s="62" t="s">
-        <v>72</v>
+      <c r="L16" s="41"/>
+      <c r="M16" s="42" t="s">
+        <v>52</v>
       </c>
       <c r="N16" s="13" t="s">
         <v>21</v>
       </c>
       <c r="O16" s="17"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="18"/>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
@@ -3496,135 +3363,112 @@
       <c r="N17" s="19"/>
       <c r="O17" s="20"/>
     </row>
-    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="41"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41"/>
-      <c r="P18" s="41"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="50"/>
+    <row r="18" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="60"/>
       <c r="L19" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="M19" s="64" t="s">
+      <c r="M19" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="N19" s="65"/>
-      <c r="O19" s="66"/>
-    </row>
-    <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="52"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="54"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="46"/>
+    </row>
+    <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="32"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="34"/>
       <c r="L20" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="M20" s="56" t="s">
+      <c r="M20" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="N20" s="41"/>
-      <c r="O20" s="60"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O20" s="40"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="16"/>
-      <c r="C21" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="29"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="H21" s="29"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="55"/>
+      <c r="C21" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="62"/>
+      <c r="E21" s="63"/>
+      <c r="G21" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="62"/>
+      <c r="I21" s="63"/>
+      <c r="J21" s="35"/>
       <c r="L21" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="56" t="s">
+      <c r="M21" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="N21" s="41"/>
-      <c r="O21" s="60"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O21" s="40"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="16"/>
-      <c r="C22" s="57" t="s">
+      <c r="C22" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="67" t="s">
-        <v>74</v>
-      </c>
-      <c r="E22" s="68" t="s">
+      <c r="D22" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="41"/>
-      <c r="G22" s="57" t="s">
+      <c r="G22" s="37" t="s">
         <v>18</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="I22" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="I22" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="J22" s="55"/>
+      <c r="J22" s="35"/>
       <c r="L22" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="M22" s="56" t="s">
+      <c r="M22" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="N22" s="41"/>
-      <c r="O22" s="60"/>
-    </row>
-    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O22" s="40"/>
+    </row>
+    <row r="23" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="16"/>
-      <c r="C23" s="59" t="s">
+      <c r="C23" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="60" t="s">
+      <c r="D23" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="41"/>
-      <c r="G23" s="61" t="s">
+      <c r="G23" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="62" t="s">
-        <v>68</v>
+      <c r="H23" s="42" t="s">
+        <v>48</v>
       </c>
       <c r="I23" s="13" t="s">
         <v>23</v>
@@ -3633,60 +3477,52 @@
       <c r="L23" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M23" s="56" t="s">
+      <c r="M23" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="N23" s="41"/>
-      <c r="O23" s="60"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O23" s="40"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="16"/>
-      <c r="C24" s="59" t="s">
+      <c r="C24" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="60" t="s">
+      <c r="D24" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="41"/>
       <c r="J24" s="17"/>
       <c r="L24" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M24" s="56" t="s">
+      <c r="M24" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="N24" s="41"/>
-      <c r="O24" s="60"/>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O24" s="40"/>
+    </row>
+    <row r="25" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="16"/>
-      <c r="C25" s="61" t="s">
+      <c r="C25" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="63" t="s">
-        <v>61</v>
+      <c r="D25" s="43" t="s">
+        <v>41</v>
       </c>
       <c r="E25" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
       <c r="J25" s="17"/>
       <c r="L25" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="M25" s="56" t="s">
+      <c r="M25" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="N25" s="41"/>
-      <c r="O25" s="60"/>
-    </row>
-    <row r="26" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O25" s="40"/>
+    </row>
+    <row r="26" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="18"/>
       <c r="C26" s="19"/>
       <c r="D26" s="19"/>
@@ -3699,10 +3535,10 @@
       <c r="L26" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="M26" s="62" t="s">
+      <c r="M26" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="N26" s="62"/>
+      <c r="N26" s="42"/>
       <c r="O26" s="13"/>
     </row>
     <row r="45" spans="4:6" x14ac:dyDescent="0.25">
@@ -3717,16 +3553,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C4:E4"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="B19:J19"/>
     <mergeCell ref="L10:N10"/>
     <mergeCell ref="G10:I10"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3734,6 +3570,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9aa52738-098e-4708-8617-ce06467393c8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1a6651db-12cd-4eb5-b959-f50a242d34d0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100538F8BF2EAF0F24DAD55241486BE0DC3" ma:contentTypeVersion="10" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="47b95f5122c676a34656c999c028f3a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9aa52738-098e-4708-8617-ce06467393c8" xmlns:ns3="1a6651db-12cd-4eb5-b959-f50a242d34d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3d9d3384b688ca0872a68b40f5fcd7e7" ns2:_="" ns3:_="">
     <xsd:import namespace="9aa52738-098e-4708-8617-ce06467393c8"/>
@@ -3922,27 +3778,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E8FBBE8-3EE7-4BC9-BBE8-BBE3A5C70E4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="9aa52738-098e-4708-8617-ce06467393c8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a6651db-12cd-4eb5-b959-f50a242d34d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9aa52738-098e-4708-8617-ce06467393c8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1a6651db-12cd-4eb5-b959-f50a242d34d0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D54F1F7C-6C5A-4B41-B8A4-6F03048D2C4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6669C33B-A46E-4583-B6E4-A0E35CC23870}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3959,29 +3820,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D54F1F7C-6C5A-4B41-B8A4-6F03048D2C4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E8FBBE8-3EE7-4BC9-BBE8-BBE3A5C70E4C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="9aa52738-098e-4708-8617-ce06467393c8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a6651db-12cd-4eb5-b959-f50a242d34d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Yhtenäistetty koodia, tarkistettu H2 ajolla koodin toiminta ja korjattu virheet sen perusteella
</commit_message>
<xml_diff>
--- a/Tietokannan suunnittelu.xlsx
+++ b/Tietokannan suunnittelu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickl\Desktop\TicketGuru\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickl\Desktop\Ohjelmistoprojekti\TicketGuru\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9133F710-44DD-439A-ACAF-99F15F3F317F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6421AC-A94D-411A-92A3-F0CD5D30AACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="870" windowWidth="17940" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="2205" windowWidth="17940" windowHeight="15570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toinen versio" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="56">
   <si>
     <t>PK</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>appUserId</t>
+  </si>
+  <si>
+    <t>postalcode</t>
   </si>
 </sst>
 </file>
@@ -784,6 +787,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -801,15 +813,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2572,8 +2575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2ADD925-C497-4A11-984D-016215FEC5E0}">
   <dimension ref="B1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J25" sqref="A1:XFD1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2781,7 +2784,7 @@
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
@@ -2889,7 +2892,7 @@
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="D22" t="s">
         <v>19</v>
@@ -3012,8 +3015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77066A0C-FE6B-41C8-82EA-ABF9313DC4DB}">
   <dimension ref="B2:O46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3041,22 +3044,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="57"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="60"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="21"/>
@@ -3076,16 +3079,16 @@
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="16"/>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="63"/>
-      <c r="G4" s="61" t="s">
+      <c r="D4" s="56"/>
+      <c r="E4" s="57"/>
+      <c r="G4" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="62"/>
-      <c r="I4" s="63"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="57"/>
       <c r="J4" s="29"/>
       <c r="O4" s="17"/>
     </row>
@@ -3166,11 +3169,11 @@
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="16"/>
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="63"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="57"/>
       <c r="G10" s="64" t="s">
         <v>30</v>
       </c>
@@ -3178,11 +3181,11 @@
       <c r="I10" s="66"/>
       <c r="J10" s="31"/>
       <c r="K10" s="29"/>
-      <c r="L10" s="61" t="s">
+      <c r="L10" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="M10" s="62"/>
-      <c r="N10" s="63"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="57"/>
       <c r="O10" s="17"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
@@ -3280,7 +3283,7 @@
         <v>20</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="I14" s="40" t="s">
         <v>19</v>
@@ -3365,17 +3368,17 @@
     </row>
     <row r="18" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="60"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="63"/>
       <c r="L19" s="10" t="s">
         <v>0</v>
       </c>
@@ -3405,16 +3408,16 @@
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="16"/>
-      <c r="C21" s="61" t="s">
+      <c r="C21" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="62"/>
-      <c r="E21" s="63"/>
-      <c r="G21" s="61" t="s">
+      <c r="D21" s="56"/>
+      <c r="E21" s="57"/>
+      <c r="G21" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="62"/>
-      <c r="I21" s="63"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="57"/>
       <c r="J21" s="35"/>
       <c r="L21" s="11" t="s">
         <v>4</v>
@@ -3570,26 +3573,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9aa52738-098e-4708-8617-ce06467393c8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1a6651db-12cd-4eb5-b959-f50a242d34d0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100538F8BF2EAF0F24DAD55241486BE0DC3" ma:contentTypeVersion="10" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="47b95f5122c676a34656c999c028f3a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9aa52738-098e-4708-8617-ce06467393c8" xmlns:ns3="1a6651db-12cd-4eb5-b959-f50a242d34d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3d9d3384b688ca0872a68b40f5fcd7e7" ns2:_="" ns3:_="">
     <xsd:import namespace="9aa52738-098e-4708-8617-ce06467393c8"/>
@@ -3778,32 +3761,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E8FBBE8-3EE7-4BC9-BBE8-BBE3A5C70E4C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="9aa52738-098e-4708-8617-ce06467393c8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a6651db-12cd-4eb5-b959-f50a242d34d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D54F1F7C-6C5A-4B41-B8A4-6F03048D2C4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9aa52738-098e-4708-8617-ce06467393c8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1a6651db-12cd-4eb5-b959-f50a242d34d0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6669C33B-A46E-4583-B6E4-A0E35CC23870}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3820,4 +3798,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D54F1F7C-6C5A-4B41-B8A4-6F03048D2C4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E8FBBE8-3EE7-4BC9-BBE8-BBE3A5C70E4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="9aa52738-098e-4708-8617-ce06467393c8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a6651db-12cd-4eb5-b959-f50a242d34d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Poistettu cities ja tehty siitä muutokset
</commit_message>
<xml_diff>
--- a/Tietokannan suunnittelu.xlsx
+++ b/Tietokannan suunnittelu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickl\Desktop\Ohjelmistoprojekti\TicketGuru\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6421AC-A94D-411A-92A3-F0CD5D30AACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3EE57F-EF95-4AD0-9E1C-91AE53C05D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2205" windowWidth="17940" windowHeight="15570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="2205" windowWidth="28665" windowHeight="17070" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toinen versio" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="53">
   <si>
     <t>PK</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Postcodes</t>
   </si>
   <si>
-    <t>Cities</t>
-  </si>
-  <si>
     <t>Usernames</t>
   </si>
   <si>
@@ -147,18 +144,9 @@
     <t>price</t>
   </si>
   <si>
-    <t>postalCode</t>
-  </si>
-  <si>
     <t>postOffice</t>
   </si>
   <si>
-    <t>cityId</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -205,6 +193,9 @@
   </si>
   <si>
     <t>postalcode</t>
+  </si>
+  <si>
+    <t>Tekstikenttä, 5 merkkiä</t>
   </si>
 </sst>
 </file>
@@ -909,15 +900,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>676272</xdr:colOff>
+      <xdr:colOff>676271</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1235349</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:colOff>1140098</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -932,66 +923,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="676272" y="2457449"/>
-          <a:ext cx="559077" cy="1609725"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightBracket">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="fi-FI" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>866774</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1235348</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Right Bracket 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE6A8026-2936-4013-9CDB-BB17F61E06B8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="866774" y="2657475"/>
-          <a:ext cx="368574" cy="619126"/>
+          <a:off x="676271" y="2609849"/>
+          <a:ext cx="463827" cy="800101"/>
         </a:xfrm>
         <a:prstGeom prst="rightBracket">
           <a:avLst/>
@@ -1192,9 +1125,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1581830</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>102577</xdr:rowOff>
+      <xdr:colOff>1575289</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>109903</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1209,59 +1142,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2976563" y="1671017"/>
-          <a:ext cx="1581830" cy="586591"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050" cmpd="sng"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>102577</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1581830</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>102577</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="12" name="Straight Connector 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7850C63B-2F09-4DC6-A432-0788F746461F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2976563" y="2460015"/>
-          <a:ext cx="1581830" cy="0"/>
+          <a:off x="2542442" y="2033700"/>
+          <a:ext cx="1575289" cy="398838"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1339,15 +1221,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>398859</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>99392</xdr:rowOff>
+      <xdr:colOff>386952</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>93440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>89297</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1362,8 +1244,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6828234" y="1671017"/>
-          <a:ext cx="1583532" cy="800721"/>
+          <a:off x="5732858" y="1867471"/>
+          <a:ext cx="1440658" cy="186357"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1397,8 +1279,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>99392</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>89296</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1413,8 +1295,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6828234" y="700088"/>
-          <a:ext cx="1583532" cy="970929"/>
+          <a:off x="5744765" y="1081088"/>
+          <a:ext cx="1428751" cy="175021"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1442,13 +1324,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>105455</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>680</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1495,13 +1377,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1229814</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>151667</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>152664</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>151667</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1563,13 +1445,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>494475</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1630,150 +1512,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1257300</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>180150</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="TextBox 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B950F64-9593-4789-A434-E9916468D2B9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3790950" y="2809875"/>
-          <a:ext cx="504000" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fi-FI" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="E6EDF3"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>484950</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="TextBox 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{259A5434-D2D3-4E20-AD30-E136DDE96536}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2514600" y="2790825"/>
-          <a:ext cx="504000" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fi-FI" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="E6EDF3"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>1..*</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
       <xdr:colOff>1238250</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>161100</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2038,15 +1784,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>816768</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>36910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>208725</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>292068</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>27385</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2061,8 +1807,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6886575" y="2781300"/>
-          <a:ext cx="504000" cy="190500"/>
+          <a:off x="6960393" y="1810941"/>
+          <a:ext cx="505191" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2106,15 +1852,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>602456</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>53578</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>256350</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>77756</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>53577</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2129,8 +1875,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6934200" y="1981200"/>
-          <a:ext cx="504000" cy="190500"/>
+          <a:off x="6746081" y="827484"/>
+          <a:ext cx="505191" cy="202406"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2241,16 +1987,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>366713</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>113475</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>71803</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>73818</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2265,8 +2011,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5762625" y="1828800"/>
-          <a:ext cx="504000" cy="190500"/>
+          <a:off x="5712619" y="1657349"/>
+          <a:ext cx="502809" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2576,7 +2322,7 @@
   <dimension ref="B1:M38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2609,7 +2355,7 @@
       <c r="D2" s="51"/>
       <c r="E2" s="3"/>
       <c r="F2" s="49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2" s="50"/>
       <c r="H2" s="51"/>
@@ -2625,7 +2371,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -2634,7 +2380,7 @@
         <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H3" t="s">
         <v>6</v>
@@ -2643,7 +2389,7 @@
         <v>18</v>
       </c>
       <c r="K3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L3" t="s">
         <v>6</v>
@@ -2654,7 +2400,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -2663,7 +2409,7 @@
         <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H4" t="s">
         <v>8</v>
@@ -2672,7 +2418,7 @@
         <v>10</v>
       </c>
       <c r="K4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -2683,7 +2429,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -2692,7 +2438,7 @@
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s">
         <v>8</v>
@@ -2701,7 +2447,7 @@
         <v>10</v>
       </c>
       <c r="K5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L5" t="s">
         <v>4</v>
@@ -2712,7 +2458,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -2723,7 +2469,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -2732,7 +2478,7 @@
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -2741,7 +2487,7 @@
     <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="52" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="53"/>
       <c r="D10" s="54"/>
@@ -2751,7 +2497,7 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
@@ -2762,7 +2508,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -2773,7 +2519,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>17</v>
@@ -2784,28 +2530,19 @@
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="53"/>
       <c r="D17" s="54"/>
@@ -2815,10 +2552,10 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2826,13 +2563,13 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G19" s="50"/>
       <c r="H19" s="51"/>
@@ -2842,12 +2579,12 @@
       <c r="K19" s="50"/>
       <c r="L19" s="51"/>
     </row>
-    <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F20" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G20" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H20" t="s">
         <v>22</v>
@@ -2856,23 +2593,18 @@
         <v>18</v>
       </c>
       <c r="K20" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="L20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="53"/>
-      <c r="D21" s="54"/>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H21" t="s">
         <v>23</v>
@@ -2881,41 +2613,21 @@
         <v>10</v>
       </c>
       <c r="K21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L21" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" t="s">
-        <v>19</v>
-      </c>
       <c r="F22" t="s">
         <v>20</v>
       </c>
       <c r="G22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H22" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2996,11 +2708,10 @@
       <c r="E38" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
     <mergeCell ref="J19:L19"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B21:D21"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="F19:H19"/>
@@ -3013,10 +2724,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77066A0C-FE6B-41C8-82EA-ABF9313DC4DB}">
-  <dimension ref="B2:O46"/>
+  <dimension ref="B2:O43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3024,17 +2735,17 @@
     <col min="1" max="1" width="9.140625" style="7"/>
     <col min="2" max="2" width="4.5703125" style="7" customWidth="1"/>
     <col min="3" max="3" width="4.140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.7109375" style="7" customWidth="1"/>
     <col min="7" max="7" width="4.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="7" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" style="7" customWidth="1"/>
-    <col min="12" max="12" width="5" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4.42578125" style="7" customWidth="1"/>
     <col min="16" max="16" width="4.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
@@ -3045,7 +2756,7 @@
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="59"/>
       <c r="D2" s="59"/>
@@ -3085,20 +2796,20 @@
       <c r="D4" s="56"/>
       <c r="E4" s="57"/>
       <c r="G4" s="55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" s="56"/>
       <c r="I4" s="57"/>
       <c r="J4" s="29"/>
       <c r="O4" s="17"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="16"/>
       <c r="C5" s="37" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="38" t="s">
         <v>6</v>
@@ -3107,7 +2818,7 @@
         <v>18</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I5" s="38" t="s">
         <v>6</v>
@@ -3120,7 +2831,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="40" t="s">
         <v>23</v>
@@ -3129,11 +2840,16 @@
         <v>20</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I6" s="40" t="s">
         <v>8</v>
       </c>
+      <c r="L6" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="56"/>
+      <c r="N6" s="57"/>
       <c r="O6" s="17"/>
     </row>
     <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3142,7 +2858,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>4</v>
@@ -3151,20 +2867,52 @@
         <v>20</v>
       </c>
       <c r="H7" s="43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>8</v>
       </c>
+      <c r="L7" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="38" t="s">
+        <v>6</v>
+      </c>
       <c r="O7" s="17"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="16"/>
       <c r="F8" s="29"/>
+      <c r="L8" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N8" s="40" t="s">
+        <v>16</v>
+      </c>
       <c r="O8" s="17"/>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="16"/>
+      <c r="G9" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="65"/>
+      <c r="I9" s="66"/>
+      <c r="L9" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" s="40" t="s">
+        <v>12</v>
+      </c>
       <c r="O9" s="17"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
@@ -3174,18 +2922,26 @@
       </c>
       <c r="D10" s="56"/>
       <c r="E10" s="57"/>
-      <c r="G10" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="65"/>
-      <c r="I10" s="66"/>
+      <c r="G10" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="38" t="s">
+        <v>6</v>
+      </c>
       <c r="J10" s="31"/>
       <c r="K10" s="29"/>
-      <c r="L10" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="M10" s="56"/>
-      <c r="N10" s="57"/>
+      <c r="L10" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" s="40" t="s">
+        <v>8</v>
+      </c>
       <c r="O10" s="17"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
@@ -3194,28 +2950,28 @@
         <v>18</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E11" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="L11" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="M11" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="N11" s="38" t="s">
-        <v>6</v>
+      <c r="G11" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="N11" s="40" t="s">
+        <v>8</v>
       </c>
       <c r="O11" s="17"/>
     </row>
@@ -3225,7 +2981,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>17</v>
@@ -3234,338 +2990,248 @@
         <v>10</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I12" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="M12" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="N12" s="40" t="s">
-        <v>16</v>
+      <c r="L12" s="41"/>
+      <c r="M12" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="O12" s="17"/>
     </row>
     <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="16"/>
-      <c r="G13" s="39" t="s">
+      <c r="G13" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="O13" s="17"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="20"/>
+    </row>
+    <row r="15" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="63"/>
+      <c r="L16" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="N16" s="45"/>
+      <c r="O16" s="46"/>
+    </row>
+    <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="32"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="34"/>
+      <c r="L17" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="O17" s="40"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="16"/>
+      <c r="C18" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="56"/>
+      <c r="E18" s="57"/>
+      <c r="G18" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="56"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="35"/>
+      <c r="L18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="O18" s="40"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="16"/>
+      <c r="C19" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="35"/>
+      <c r="L19" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="M19" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="O19" s="40"/>
+    </row>
+    <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="16"/>
+      <c r="C20" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I13" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="L13" s="39" t="s">
+      <c r="D20" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="M13" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="N13" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="O13" s="17"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
-      <c r="C14" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="65"/>
-      <c r="E14" s="66"/>
-      <c r="G14" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="I14" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="L14" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="M14" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="N14" s="40" t="s">
+      <c r="H20" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="17"/>
+      <c r="L20" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="O14" s="17"/>
-    </row>
-    <row r="15" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="16"/>
-      <c r="C15" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="L15" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="N15" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="O15" s="17"/>
-    </row>
-    <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="16"/>
-      <c r="C16" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L16" s="41"/>
-      <c r="M16" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="N16" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="O16" s="17"/>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="20"/>
-    </row>
-    <row r="18" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="61" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="62"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="63"/>
-      <c r="L19" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="M19" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="N19" s="45"/>
-      <c r="O19" s="46"/>
-    </row>
-    <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="32"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="34"/>
-      <c r="L20" s="11" t="s">
-        <v>2</v>
-      </c>
       <c r="M20" s="36" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="O20" s="40"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="16"/>
-      <c r="C21" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="56"/>
-      <c r="E21" s="57"/>
-      <c r="G21" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="H21" s="56"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="35"/>
+      <c r="C21" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="17"/>
       <c r="L21" s="11" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="M21" s="36" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="O21" s="40"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="16"/>
-      <c r="C22" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="48" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="I22" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="J22" s="35"/>
+      <c r="C22" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="17"/>
       <c r="L22" s="11" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="M22" s="36" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="O22" s="40"/>
     </row>
     <row r="23" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="16"/>
-      <c r="C23" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J23" s="17"/>
-      <c r="L23" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="M23" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="O23" s="40"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="16"/>
-      <c r="C24" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="J24" s="17"/>
-      <c r="L24" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="M24" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="O24" s="40"/>
-    </row>
-    <row r="25" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="16"/>
-      <c r="C25" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="J25" s="17"/>
-      <c r="L25" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="M25" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="O25" s="40"/>
-    </row>
-    <row r="26" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="20"/>
-      <c r="L26" s="12" t="s">
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="20"/>
+      <c r="L23" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="M26" s="42" t="s">
+      <c r="M23" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="N26" s="42"/>
-      <c r="O26" s="13"/>
-    </row>
-    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-    </row>
-    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="13"/>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="G21:I21"/>
+  <mergeCells count="9">
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="G18:I18"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="B2:O2"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="B16:J16"/>
     <mergeCell ref="G4:I4"/>
-    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="L6:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3573,6 +3239,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9aa52738-098e-4708-8617-ce06467393c8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1a6651db-12cd-4eb5-b959-f50a242d34d0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100538F8BF2EAF0F24DAD55241486BE0DC3" ma:contentTypeVersion="10" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="47b95f5122c676a34656c999c028f3a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9aa52738-098e-4708-8617-ce06467393c8" xmlns:ns3="1a6651db-12cd-4eb5-b959-f50a242d34d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3d9d3384b688ca0872a68b40f5fcd7e7" ns2:_="" ns3:_="">
     <xsd:import namespace="9aa52738-098e-4708-8617-ce06467393c8"/>
@@ -3761,27 +3447,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E8FBBE8-3EE7-4BC9-BBE8-BBE3A5C70E4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="9aa52738-098e-4708-8617-ce06467393c8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a6651db-12cd-4eb5-b959-f50a242d34d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9aa52738-098e-4708-8617-ce06467393c8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1a6651db-12cd-4eb5-b959-f50a242d34d0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D54F1F7C-6C5A-4B41-B8A4-6F03048D2C4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6669C33B-A46E-4583-B6E4-A0E35CC23870}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3798,29 +3489,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D54F1F7C-6C5A-4B41-B8A4-6F03048D2C4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E8FBBE8-3EE7-4BC9-BBE8-BBE3A5C70E4C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="9aa52738-098e-4708-8617-ce06467393c8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a6651db-12cd-4eb5-b959-f50a242d34d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Tehty viimeistelyt ja korjaukset edellisen viikon sprinttiin
</commit_message>
<xml_diff>
--- a/Tietokannan suunnittelu.xlsx
+++ b/Tietokannan suunnittelu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://haagahelia.sharepoint.com/teams/Ohjelmistoprojekti1-Tiimi/Jaetut asiakirjat/General/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickl\Desktop\Ohjelmistoprojekti\TicketGuru\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{D30A7D45-AD24-43D7-9701-3842121119DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9D3987F-B05B-45CC-B0A9-6427B27F70F0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5538A36-EA5A-47F4-8A8E-C0311FCB553D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1575" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26535" yWindow="1695" windowWidth="25350" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2.0" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="60">
   <si>
     <t>Tickets</t>
   </si>
@@ -204,9 +204,6 @@
     <t>amount</t>
   </si>
   <si>
-    <t>check</t>
-  </si>
-  <si>
     <t>transactionDate</t>
   </si>
   <si>
@@ -214,6 +211,12 @@
   </si>
   <si>
     <t>eventTime</t>
+  </si>
+  <si>
+    <t>isChecked</t>
+  </si>
+  <si>
+    <t>roleName</t>
   </si>
 </sst>
 </file>
@@ -633,6 +636,15 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -640,15 +652,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3244,8 +3247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDD9BD3-2EDA-4A24-8766-7E2FFAA8363C}">
   <dimension ref="B1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3271,22 +3274,22 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="50"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="47"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="42"/>
@@ -3306,21 +3309,21 @@
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="38"/>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="47"/>
-      <c r="G4" s="45" t="s">
+      <c r="D4" s="49"/>
+      <c r="E4" s="50"/>
+      <c r="G4" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="47"/>
-      <c r="L4" s="45" t="s">
+      <c r="H4" s="49"/>
+      <c r="I4" s="50"/>
+      <c r="L4" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="M4" s="46"/>
-      <c r="N4" s="47"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="50"/>
       <c r="O4" s="27"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
@@ -3394,7 +3397,7 @@
         <v>16</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L7" s="26" t="s">
         <v>14</v>
@@ -3409,11 +3412,11 @@
     </row>
     <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="38"/>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
       <c r="F8" s="16"/>
       <c r="G8" s="28" t="s">
         <v>9</v>
@@ -3448,7 +3451,7 @@
       </c>
       <c r="L9" s="28"/>
       <c r="M9" s="30" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N9" s="7" t="s">
         <v>50</v>
@@ -3466,11 +3469,11 @@
       <c r="E10" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="45" t="s">
+      <c r="G10" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="46"/>
-      <c r="I10" s="47"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="50"/>
       <c r="J10" s="18"/>
       <c r="K10" s="16"/>
       <c r="O10" s="27"/>
@@ -3497,11 +3500,11 @@
       </c>
       <c r="J11" s="18"/>
       <c r="K11" s="16"/>
-      <c r="L11" s="45" t="s">
+      <c r="L11" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="M11" s="46"/>
-      <c r="N11" s="47"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="50"/>
       <c r="O11" s="27"/>
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3541,7 +3544,7 @@
         <v>9</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I13" s="27" t="s">
         <v>26</v>
@@ -3563,7 +3566,7 @@
         <v>9</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I14" s="27" t="s">
         <v>26</v>
@@ -3572,7 +3575,7 @@
         <v>9</v>
       </c>
       <c r="M14" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N14" s="7" t="s">
         <v>26</v>
@@ -3634,23 +3637,23 @@
     </row>
     <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="50"/>
-      <c r="L20" s="48" t="s">
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="47"/>
+      <c r="L20" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="M20" s="49"/>
-      <c r="N20" s="49"/>
-      <c r="O20" s="50"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="46"/>
+      <c r="O20" s="47"/>
     </row>
     <row r="21" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="36"/>
@@ -3672,16 +3675,16 @@
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="38"/>
-      <c r="C22" s="45" t="s">
+      <c r="C22" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="46"/>
-      <c r="E22" s="47"/>
-      <c r="G22" s="45" t="s">
+      <c r="D22" s="49"/>
+      <c r="E22" s="50"/>
+      <c r="G22" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="H22" s="46"/>
-      <c r="I22" s="47"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="50"/>
       <c r="J22" s="39"/>
       <c r="L22" s="5" t="s">
         <v>36</v>
@@ -3735,7 +3738,7 @@
         <v>9</v>
       </c>
       <c r="H24" s="29" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="I24" s="7" t="s">
         <v>13</v>
@@ -3829,17 +3832,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="B2:O2"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="L4:N4"/>
     <mergeCell ref="G10:I10"/>
     <mergeCell ref="L20:O20"/>
     <mergeCell ref="B20:J20"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="G22:I22"/>
     <mergeCell ref="L11:N11"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="L4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3915,16 +3918,16 @@
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="47"/>
-      <c r="G4" s="45" t="s">
+      <c r="D4" s="49"/>
+      <c r="E4" s="50"/>
+      <c r="G4" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="47"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="50"/>
       <c r="J4" s="16"/>
       <c r="O4" s="11"/>
     </row>
@@ -3970,11 +3973,11 @@
       <c r="I6" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="45" t="s">
+      <c r="L6" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="46"/>
-      <c r="N6" s="47"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="50"/>
       <c r="O6" s="11"/>
     </row>
     <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4024,11 +4027,11 @@
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="10"/>
-      <c r="G9" s="48" t="s">
+      <c r="G9" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="49"/>
-      <c r="I9" s="50"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="47"/>
       <c r="L9" s="26" t="s">
         <v>9</v>
       </c>
@@ -4042,11 +4045,11 @@
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="47"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="50"/>
       <c r="G10" s="24" t="s">
         <v>3</v>
       </c>
@@ -4200,16 +4203,16 @@
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="46"/>
-      <c r="E18" s="47"/>
-      <c r="G18" s="45" t="s">
+      <c r="D18" s="49"/>
+      <c r="E18" s="50"/>
+      <c r="G18" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="46"/>
-      <c r="I18" s="47"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="50"/>
       <c r="J18" s="22"/>
       <c r="L18" s="5" t="s">
         <v>5</v>
@@ -4364,12 +4367,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9aa52738-098e-4708-8617-ce06467393c8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1a6651db-12cd-4eb5-b959-f50a242d34d0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4562,20 +4567,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9aa52738-098e-4708-8617-ce06467393c8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1a6651db-12cd-4eb5-b959-f50a242d34d0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D54F1F7C-6C5A-4B41-B8A4-6F03048D2C4F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E8FBBE8-3EE7-4BC9-BBE8-BBE3A5C70E4C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1a6651db-12cd-4eb5-b959-f50a242d34d0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9aa52738-098e-4708-8617-ce06467393c8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4600,18 +4612,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E8FBBE8-3EE7-4BC9-BBE8-BBE3A5C70E4C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D54F1F7C-6C5A-4B41-B8A4-6F03048D2C4F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1a6651db-12cd-4eb5-b959-f50a242d34d0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9aa52738-098e-4708-8617-ce06467393c8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
tehty päivitetty readme tiedostoa
</commit_message>
<xml_diff>
--- a/Tietokannan suunnittelu.xlsx
+++ b/Tietokannan suunnittelu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickl\Desktop\Ohjelmistoprojekti\TicketGuru\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5538A36-EA5A-47F4-8A8E-C0311FCB553D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B27DFB5-C6FB-4967-9FBF-802BF1F9E922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26535" yWindow="1695" windowWidth="25350" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16320" yWindow="1200" windowWidth="20970" windowHeight="17955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2.0" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="82">
   <si>
     <t>Tickets</t>
   </si>
@@ -195,28 +195,94 @@
     <t>Boolean</t>
   </si>
   <si>
-    <t>Transactions</t>
-  </si>
-  <si>
-    <t>transactionId</t>
-  </si>
-  <si>
     <t>amount</t>
   </si>
   <si>
-    <t>transactionDate</t>
-  </si>
-  <si>
-    <t>eventDate</t>
-  </si>
-  <si>
-    <t>eventTime</t>
-  </si>
-  <si>
-    <t>isChecked</t>
-  </si>
-  <si>
-    <t>roleName</t>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>role_id</t>
+  </si>
+  <si>
+    <t>roles</t>
+  </si>
+  <si>
+    <t>app_users</t>
+  </si>
+  <si>
+    <t>postalcodes</t>
+  </si>
+  <si>
+    <t>venues</t>
+  </si>
+  <si>
+    <t>events</t>
+  </si>
+  <si>
+    <t>role_name</t>
+  </si>
+  <si>
+    <t>post_office</t>
+  </si>
+  <si>
+    <t>venue_id</t>
+  </si>
+  <si>
+    <t>street_address</t>
+  </si>
+  <si>
+    <t>event_id</t>
+  </si>
+  <si>
+    <t>event_name</t>
+  </si>
+  <si>
+    <t>event_date</t>
+  </si>
+  <si>
+    <t>event_time</t>
+  </si>
+  <si>
+    <t>ticket_count</t>
+  </si>
+  <si>
+    <t>ticket_types</t>
+  </si>
+  <si>
+    <t>tyicket_type_id</t>
+  </si>
+  <si>
+    <t>ticket_type</t>
+  </si>
+  <si>
+    <t>ticket_id</t>
+  </si>
+  <si>
+    <t>ticket_type_id</t>
+  </si>
+  <si>
+    <t>transaction_id</t>
+  </si>
+  <si>
+    <t>is_checked</t>
+  </si>
+  <si>
+    <t>tickets</t>
+  </si>
+  <si>
+    <t>transactions</t>
+  </si>
+  <si>
+    <t>transaction_ok</t>
+  </si>
+  <si>
+    <t>transaction_date</t>
+  </si>
+  <si>
+    <t>transaction_time</t>
+  </si>
+  <si>
+    <t>C/8</t>
   </si>
 </sst>
 </file>
@@ -636,6 +702,15 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -643,15 +718,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -775,8 +841,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2381250" y="4143375"/>
-          <a:ext cx="513525" cy="190500"/>
+          <a:off x="2576262" y="4950493"/>
+          <a:ext cx="740621" cy="191002"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1851,7 +1917,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>300404</xdr:colOff>
+      <xdr:colOff>132522</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>111124</xdr:rowOff>
     </xdr:to>
@@ -1868,8 +1934,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8658590" y="1466605"/>
-          <a:ext cx="309564" cy="791307"/>
+          <a:off x="8870433" y="1470427"/>
+          <a:ext cx="257002" cy="794175"/>
         </a:xfrm>
         <a:prstGeom prst="rightBracket">
           <a:avLst/>
@@ -1904,13 +1970,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>246403</xdr:colOff>
+      <xdr:colOff>320946</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>49516</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>373801</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>59061</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>49515</xdr:rowOff>
     </xdr:to>
@@ -1927,8 +1993,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8665038" y="1214497"/>
-          <a:ext cx="376513" cy="197826"/>
+          <a:off x="8951424" y="1217364"/>
+          <a:ext cx="491833" cy="198781"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1972,15 +2038,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>197827</xdr:colOff>
+      <xdr:colOff>313783</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>117231</xdr:rowOff>
+      <xdr:rowOff>100666</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>223850</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>66480</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>49898</xdr:rowOff>
+      <xdr:rowOff>33333</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1995,8 +2061,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8616462" y="2264019"/>
-          <a:ext cx="663465" cy="320994"/>
+          <a:off x="8944261" y="2254144"/>
+          <a:ext cx="779741" cy="321950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3248,25 +3314,25 @@
   <dimension ref="B1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="5.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="4.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="1" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="4.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.85546875" style="1" customWidth="1"/>
     <col min="16" max="16" width="4.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
@@ -3274,22 +3340,22 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="47"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="42"/>
@@ -3309,21 +3375,21 @@
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="38"/>
-      <c r="C4" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="50"/>
-      <c r="G4" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="49"/>
-      <c r="I4" s="50"/>
-      <c r="L4" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="M4" s="49"/>
-      <c r="N4" s="50"/>
+      <c r="C4" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="46"/>
+      <c r="E4" s="47"/>
+      <c r="G4" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="46"/>
+      <c r="I4" s="47"/>
+      <c r="L4" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="M4" s="46"/>
+      <c r="N4" s="47"/>
       <c r="O4" s="27"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
@@ -3341,7 +3407,7 @@
         <v>3</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="I5" s="25" t="s">
         <v>7</v>
@@ -3350,7 +3416,7 @@
         <v>3</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="N5" s="25" t="s">
         <v>7</v>
@@ -3363,7 +3429,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>11</v>
@@ -3372,7 +3438,7 @@
         <v>9</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="I6" s="27" t="s">
         <v>13</v>
@@ -3381,7 +3447,7 @@
         <v>14</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="N6" s="27" t="s">
         <v>15</v>
@@ -3394,7 +3460,7 @@
         <v>14</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="I7" s="27" t="s">
         <v>15</v>
@@ -3403,7 +3469,7 @@
         <v>14</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="N7" s="27" t="s">
         <v>15</v>
@@ -3412,11 +3478,11 @@
     </row>
     <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="38"/>
-      <c r="C8" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="47"/>
+      <c r="C8" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="49"/>
+      <c r="E8" s="50"/>
       <c r="F8" s="16"/>
       <c r="G8" s="28" t="s">
         <v>9</v>
@@ -3431,7 +3497,7 @@
         <v>14</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="N8" s="27" t="s">
         <v>15</v>
@@ -3444,14 +3510,14 @@
         <v>3</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>7</v>
       </c>
       <c r="L9" s="28"/>
       <c r="M9" s="30" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="N9" s="7" t="s">
         <v>50</v>
@@ -3469,11 +3535,11 @@
       <c r="E10" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="48" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="49"/>
-      <c r="I10" s="50"/>
+      <c r="G10" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="46"/>
+      <c r="I10" s="47"/>
       <c r="J10" s="18"/>
       <c r="K10" s="16"/>
       <c r="O10" s="27"/>
@@ -3484,7 +3550,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="E11" s="27" t="s">
         <v>11</v>
@@ -3493,18 +3559,18 @@
         <v>3</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="I11" s="25" t="s">
         <v>7</v>
       </c>
       <c r="J11" s="18"/>
       <c r="K11" s="16"/>
-      <c r="L11" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="M11" s="49"/>
-      <c r="N11" s="50"/>
+      <c r="L11" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="M11" s="46"/>
+      <c r="N11" s="47"/>
       <c r="O11" s="27"/>
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3522,7 +3588,7 @@
         <v>9</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="I12" s="27" t="s">
         <v>24</v>
@@ -3531,7 +3597,7 @@
         <v>3</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="N12" s="25" t="s">
         <v>7</v>
@@ -3544,7 +3610,7 @@
         <v>9</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="I13" s="27" t="s">
         <v>26</v>
@@ -3553,32 +3619,32 @@
         <v>9</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N13" s="27" t="s">
         <v>15</v>
       </c>
       <c r="O13" s="27"/>
     </row>
-    <row r="14" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="38"/>
       <c r="G14" s="26" t="s">
         <v>9</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="I14" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="L14" s="28" t="s">
+      <c r="L14" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="M14" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="N14" s="7" t="s">
-        <v>26</v>
+      <c r="M14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N14" s="27" t="s">
+        <v>50</v>
       </c>
       <c r="O14" s="27"/>
     </row>
@@ -3588,23 +3654,41 @@
         <v>9</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="I15" s="27" t="s">
         <v>15</v>
       </c>
+      <c r="L15" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N15" s="27" t="s">
+        <v>49</v>
+      </c>
       <c r="O15" s="27"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="38"/>
       <c r="G16" s="26" t="s">
         <v>14</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="I16" s="27" t="s">
         <v>15</v>
+      </c>
+      <c r="L16" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="O16" s="27"/>
     </row>
@@ -3637,23 +3721,23 @@
     </row>
     <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="47"/>
-      <c r="L20" s="45" t="s">
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="50"/>
+      <c r="L20" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="M20" s="46"/>
-      <c r="N20" s="46"/>
-      <c r="O20" s="47"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="50"/>
     </row>
     <row r="21" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="36"/>
@@ -3675,16 +3759,16 @@
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="38"/>
-      <c r="C22" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="49"/>
-      <c r="E22" s="50"/>
-      <c r="G22" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" s="49"/>
-      <c r="I22" s="50"/>
+      <c r="C22" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="46"/>
+      <c r="E22" s="47"/>
+      <c r="G22" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" s="46"/>
+      <c r="I22" s="47"/>
       <c r="J22" s="39"/>
       <c r="L22" s="5" t="s">
         <v>36</v>
@@ -3700,7 +3784,7 @@
         <v>3</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="E23" s="35" t="s">
         <v>7</v>
@@ -3709,7 +3793,7 @@
         <v>3</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="I23" s="25" t="s">
         <v>7</v>
@@ -3738,7 +3822,7 @@
         <v>9</v>
       </c>
       <c r="H24" s="29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I24" s="7" t="s">
         <v>13</v>
@@ -3778,7 +3862,7 @@
         <v>14</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>15</v>
@@ -3832,17 +3916,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="L4:N4"/>
     <mergeCell ref="G10:I10"/>
     <mergeCell ref="L20:O20"/>
     <mergeCell ref="B20:J20"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="G22:I22"/>
     <mergeCell ref="L11:N11"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="B2:O2"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="L4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3918,16 +4002,16 @@
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="50"/>
-      <c r="G4" s="48" t="s">
+      <c r="D4" s="46"/>
+      <c r="E4" s="47"/>
+      <c r="G4" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="49"/>
-      <c r="I4" s="50"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="47"/>
       <c r="J4" s="16"/>
       <c r="O4" s="11"/>
     </row>
@@ -3973,11 +4057,11 @@
       <c r="I6" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="48" t="s">
+      <c r="L6" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="49"/>
-      <c r="N6" s="50"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="47"/>
       <c r="O6" s="11"/>
     </row>
     <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4027,11 +4111,11 @@
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="10"/>
-      <c r="G9" s="45" t="s">
+      <c r="G9" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="46"/>
-      <c r="I9" s="47"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="50"/>
       <c r="L9" s="26" t="s">
         <v>9</v>
       </c>
@@ -4045,11 +4129,11 @@
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="50"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="47"/>
       <c r="G10" s="24" t="s">
         <v>3</v>
       </c>
@@ -4203,16 +4287,16 @@
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="49"/>
-      <c r="E18" s="50"/>
-      <c r="G18" s="48" t="s">
+      <c r="D18" s="46"/>
+      <c r="E18" s="47"/>
+      <c r="G18" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="49"/>
-      <c r="I18" s="50"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="47"/>
       <c r="J18" s="22"/>
       <c r="L18" s="5" t="s">
         <v>5</v>
@@ -4367,14 +4451,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9aa52738-098e-4708-8617-ce06467393c8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1a6651db-12cd-4eb5-b959-f50a242d34d0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4567,27 +4649,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9aa52738-098e-4708-8617-ce06467393c8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1a6651db-12cd-4eb5-b959-f50a242d34d0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E8FBBE8-3EE7-4BC9-BBE8-BBE3A5C70E4C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D54F1F7C-6C5A-4B41-B8A4-6F03048D2C4F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1a6651db-12cd-4eb5-b959-f50a242d34d0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9aa52738-098e-4708-8617-ce06467393c8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4612,9 +4687,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D54F1F7C-6C5A-4B41-B8A4-6F03048D2C4F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E8FBBE8-3EE7-4BC9-BBE8-BBE3A5C70E4C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1a6651db-12cd-4eb5-b959-f50a242d34d0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9aa52738-098e-4708-8617-ce06467393c8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>